<commit_message>
getting planedTarget efficiency from database
</commit_message>
<xml_diff>
--- a/src/assets/files/DailyPlanSample.xlsx
+++ b/src/assets/files/DailyPlanSample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udiths\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahithr\Desktop\Softmatter-PMS-frontend\softmatter-pms\src\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFFF7179-3776-431E-8445-6414FF1CC31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D4FA12-A8E8-41C5-BDAB-ED716121B7BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
   <si>
     <t>date</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>R623-724(R1)</t>
+  </si>
+  <si>
+    <t>plannedTarget</t>
   </si>
 </sst>
 </file>
@@ -177,9 +180,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -217,7 +220,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -323,7 +326,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,7 +468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -473,25 +476,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -519,8 +522,11 @@
       <c r="I1" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45481</v>
       </c>
@@ -548,8 +554,11 @@
       <c r="I2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45481</v>
       </c>
@@ -577,8 +586,11 @@
       <c r="I3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45482</v>
       </c>
@@ -606,8 +618,11 @@
       <c r="I4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45482</v>
       </c>
@@ -635,8 +650,11 @@
       <c r="I5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45483</v>
       </c>
@@ -665,7 +683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45483</v>
       </c>
@@ -694,7 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45484</v>
       </c>
@@ -723,7 +741,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45484</v>
       </c>
@@ -752,7 +770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45485</v>
       </c>
@@ -781,7 +799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45485</v>
       </c>
@@ -810,7 +828,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45486</v>
       </c>
@@ -839,7 +857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45486</v>
       </c>
@@ -868,22 +886,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
     </row>
   </sheetData>

</xml_diff>